<commit_message>
added Procfile for running gunicorn server'
</commit_message>
<xml_diff>
--- a/todo_setup.xlsx
+++ b/todo_setup.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>conda create -n todo python=3.6</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>type heroku login , follow web popup login</t>
+  </si>
+  <si>
+    <t>close and save this excel</t>
+  </si>
+  <si>
+    <t>git init</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t>git commit -m "first upload"</t>
+  </si>
+  <si>
+    <t>heroku create crudtasklist</t>
+  </si>
+  <si>
+    <t>git remote -v (shows git paths on remote server)</t>
   </si>
 </sst>
 </file>
@@ -452,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -561,6 +579,36 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>